<commit_message>
Actualizacion metamodelo, participantes y financiero
</commit_message>
<xml_diff>
--- a/HT-6/Optica BAC-04-Catálogo de participantes.xlsx
+++ b/HT-6/Optica BAC-04-Catálogo de participantes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chech\Documents\GitHub\p3\arquiemp\HT-5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chech\Documents\GitHub\p3\arquiemp\HT-6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FBF156-1E8D-4C9A-A6BB-7EFFB3345745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEF39BF-4D4B-4B78-9315-7AD782F59EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="14370" windowHeight="7270" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-04" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -57,10 +57,22 @@
     <t>Vendedor</t>
   </si>
   <si>
-    <t>Supervisor</t>
-  </si>
-  <si>
     <t>Bodeguero</t>
+  </si>
+  <si>
+    <t>Asesor Comercial</t>
+  </si>
+  <si>
+    <t>Director logístico</t>
+  </si>
+  <si>
+    <t>Empleado de recursos humanos</t>
+  </si>
+  <si>
+    <t>Gerente general</t>
+  </si>
+  <si>
+    <t>Asesor de imagen de marca</t>
   </si>
 </sst>
 </file>
@@ -129,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -139,13 +151,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -510,8 +518,8 @@
       <c r="A7" s="4">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -523,24 +531,44 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>